<commit_message>
merge translations for 4.2
</commit_message>
<xml_diff>
--- a/examples/reports/ru-ru/ChatTemplate.xlsx
+++ b/examples/reports/ru-ru/ChatTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20399"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Projects\reportgenerator\src\Cognitive.ReportGenerator\Templates\ru-ru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\bidzaar\src\etplight\backend\services\reportgenerator\src\Cognitive.ReportGenerator\Templates\ru-ru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E2F4E3-FF16-4C9E-8255-0E62C6F063F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0247F8FB-5733-4D14-9982-F316D7EDB443}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3804" yWindow="1608" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>$.CreatedCompany</t>
   </si>
   <si>
-    <t>Документ сформирован $.Now, время в документе указано в часовом поясе $.Tz</t>
-  </si>
-  <si>
     <t>Название чата / чат с ...</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Ссылка</t>
+  </si>
+  <si>
+    <t>Сформировано $.BrandName в $.Now, время в документе указано в часовом поясе $.Tz</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +127,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,9 +194,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -230,10 +233,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,7 +515,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -525,105 +531,105 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.6">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.6">
-      <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.6">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:4" ht="15.6">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.2" thickBot="1">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.6">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.6">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="12" spans="1:4" ht="15.6">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="14"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="13"/>
     </row>
     <row r="13" spans="1:4" ht="15.6">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" ht="15.6">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="15.6">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="13"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>